<commit_message>
Finished hardware map (for now)
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\git\2021-2022-LITTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256865A2-ADA2-4994-8A44-E45C83FEB0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC31166-C876-402E-8FE7-9EB6A8C3D7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>PORT</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>rotation sensor for the lift motor</t>
+  </si>
+  <si>
+    <t>Inertial</t>
+  </si>
+  <si>
+    <t>imu</t>
+  </si>
+  <si>
+    <t>Inertial sensor for odometry</t>
   </si>
 </sst>
 </file>
@@ -502,7 +511,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,6 +553,15 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">

</xml_diff>

<commit_message>
start of fork controls
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dana5\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C309C1-6B8C-44A2-B101-2FFB99F9B6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB54F991-B702-42D2-8A3D-CACAEDBD4624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10270" yWindow="1840" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>PORT</t>
   </si>
@@ -175,13 +175,40 @@
   </si>
   <si>
     <t>right_enc</t>
+  </si>
+  <si>
+    <t>imu</t>
+  </si>
+  <si>
+    <t>inertial sensor</t>
+  </si>
+  <si>
+    <t>lim</t>
+  </si>
+  <si>
+    <t>fork limit switch</t>
+  </si>
+  <si>
+    <t>Pneumatics*</t>
+  </si>
+  <si>
+    <t>Limit*</t>
+  </si>
+  <si>
+    <t>mogo_lock1</t>
+  </si>
+  <si>
+    <t>mogo_lock2</t>
+  </si>
+  <si>
+    <t>Inertial*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,6 +218,12 @@
     </font>
     <font>
       <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -217,12 +250,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,7 +616,15 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -838,16 +880,36 @@
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fork can hold mogo
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dana5\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEX\2021-2022-LITTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB54F991-B702-42D2-8A3D-CACAEDBD4624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A4A87-4798-4FE1-8538-04DB311C4726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>PORT</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>mogo_lock1</t>
-  </si>
-  <si>
-    <t>mogo_lock2</t>
   </si>
   <si>
     <t>Inertial*</t>
@@ -573,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>49</v>
@@ -904,12 +901,6 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
more fork controls, distance sensor instead of limit
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEX\2021-2022-LITTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A4A87-4798-4FE1-8538-04DB311C4726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA95A681-70AE-40E4-8548-C7A9BB71A922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6990" yWindow="2160" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,22 +183,22 @@
     <t>inertial sensor</t>
   </si>
   <si>
-    <t>lim</t>
-  </si>
-  <si>
-    <t>fork limit switch</t>
-  </si>
-  <si>
     <t>Pneumatics*</t>
   </si>
   <si>
-    <t>Limit*</t>
-  </si>
-  <si>
     <t>mogo_lock1</t>
   </si>
   <si>
     <t>Inertial*</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>detects mobile goals in fork</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>49</v>
@@ -627,6 +627,15 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -877,25 +886,17 @@
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" t="s">
-        <v>52</v>
-      </c>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fork update + vision automation (copied from BIG))
</commit_message>
<xml_diff>
--- a/hardware_map.xlsx
+++ b/hardware_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEX\2021-2022-LITTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA95A681-70AE-40E4-8548-C7A9BB71A922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7132B86-1366-416E-A598-6A0CD605E4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="2160" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>PORT</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Pneumatics*</t>
   </si>
   <si>
-    <t>mogo_lock1</t>
-  </si>
-  <si>
     <t>Inertial*</t>
   </si>
   <si>
@@ -199,6 +196,18 @@
   </si>
   <si>
     <t>Distance</t>
+  </si>
+  <si>
+    <t>mogo_locks</t>
+  </si>
+  <si>
+    <t>Vision</t>
+  </si>
+  <si>
+    <t>vis</t>
+  </si>
+  <si>
+    <t>vision sensor for mogo detection</t>
   </si>
 </sst>
 </file>
@@ -570,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,7 +623,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>49</v>
@@ -628,13 +637,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -681,6 +690,15 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -896,7 +914,7 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>